<commit_message>
Finished buzzes and rankings
</commit_message>
<xml_diff>
--- a/round_summary_mockup.xlsx
+++ b/round_summary_mockup.xlsx
@@ -8,26 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Desktop\TangStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDACA319-4032-4374-A62F-2EB8D070DCB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12B9310-BB66-404D-96B5-242DCB4D30D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Round Overview" sheetId="1" r:id="rId1"/>
     <sheet name="TeamOverview1" sheetId="2" r:id="rId2"/>
     <sheet name="TeamOverview2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>Round</t>
   </si>
@@ -86,9 +96,6 @@
     <t>matt2</t>
   </si>
   <si>
-    <t>Tossup data</t>
-  </si>
-  <si>
     <t>Tossup #</t>
   </si>
   <si>
@@ -135,6 +142,96 @@
   </si>
   <si>
     <t>Points from bonuses</t>
+  </si>
+  <si>
+    <t>HEARD</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>Myth</t>
+  </si>
+  <si>
+    <t>RELIGION</t>
+  </si>
+  <si>
+    <t>TEAM</t>
+  </si>
+  <si>
+    <t>PLAYER 1</t>
+  </si>
+  <si>
+    <t>BUZZ data</t>
+  </si>
+  <si>
+    <t>30/20/10/0</t>
+  </si>
+  <si>
+    <t>SUBCAT</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>15/10/-5/-1</t>
+  </si>
+  <si>
+    <t>Bonuses</t>
+  </si>
+  <si>
+    <t>Tossup</t>
+  </si>
+  <si>
+    <t>MISC data for processing</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Team-Player</t>
+  </si>
+  <si>
+    <t>cDepth</t>
+  </si>
+  <si>
+    <t>PPTUH</t>
+  </si>
+  <si>
+    <t>Teams heard</t>
+  </si>
+  <si>
+    <t>15's</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -5's</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>30's</t>
+  </si>
+  <si>
+    <t>20's</t>
+  </si>
+  <si>
+    <t>0's</t>
+  </si>
+  <si>
+    <t>Tossup#</t>
+  </si>
+  <si>
+    <t>Belief</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Round#</t>
   </si>
 </sst>
 </file>
@@ -178,9 +275,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -196,10 +294,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -465,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +570,7 @@
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -492,7 +586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -500,7 +594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -511,7 +605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -522,7 +616,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -533,14 +627,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -550,10 +677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F53C865-8396-45EE-8941-5FDE6F6A9B45}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,9 +691,10 @@
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -574,7 +702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -583,8 +711,26 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="T3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -603,8 +749,51 @@
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -623,8 +812,44 @@
       <c r="F5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5">
+        <v>-5</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" t="s">
+        <v>39</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -643,110 +868,35 @@
       <c r="F6">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
         <v>17</v>
       </c>
-      <c r="C10">
-        <v>-5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="J6">
+        <v>15</v>
+      </c>
+      <c r="K6" t="s">
         <v>29</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="L6" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
+      <c r="M6" t="s">
         <v>31</v>
       </c>
-      <c r="F11" t="s">
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>10</v>
+      </c>
+      <c r="Q6" t="s">
         <v>32</v>
       </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-      <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>33</v>
+      <c r="T6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -776,4 +926,156 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B046C305-1B26-4F02-8EB7-981219DD8058}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>-5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D65FB5-C856-4D3B-85FF-AD46BC353252}">
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>